<commit_message>
Homog and aligned Kitty's dfrac data. Updated tarball to GeoMicro/GeoMicro_aligned_tarball_2022-12-30.rds
</commit_message>
<xml_diff>
--- a/Data/GeoMicro/IGSN/IGSN_Key_V3.xlsx
+++ b/Data/GeoMicro/IGSN/IGSN_Key_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\EDaH\Data\GeoMicro\IGSN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A760D2C8-BC22-45FB-A243-E5170B7E40A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F4893A-C7BF-4ADD-8E5E-3F1D51EE4857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Location_data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="664">
   <si>
     <t>var</t>
   </si>
@@ -2512,7 +2512,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3227,6 +3227,9 @@
       </c>
       <c r="D13" s="6" t="s">
         <v>660</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="N13" s="19"/>
       <c r="P13" s="13"/>

</xml_diff>